<commit_message>
Started adding facial descriptions again. Added some styles to a few players. Finished positional generators.
</commit_message>
<xml_diff>
--- a/docs/Testing/2019/Randomly Generated Overall Ratings Distribution.xlsx
+++ b/docs/Testing/2019/Randomly Generated Overall Ratings Distribution.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="46">
   <si>
     <t>0 (QB)</t>
   </si>
@@ -502,7 +502,7 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1495,7 +1495,16 @@
         <v>55</v>
       </c>
       <c r="T16" s="1">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="U16" s="1">
+        <v>55</v>
+      </c>
+      <c r="V16" s="1">
+        <v>55</v>
+      </c>
+      <c r="W16" s="1">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.45">
@@ -1559,9 +1568,15 @@
       <c r="T17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
+      <c r="U17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="W17" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="18" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
@@ -1622,11 +1637,17 @@
         <v>0.11</v>
       </c>
       <c r="T18" s="4">
-        <v>0.18</v>
-      </c>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
+        <v>0.13</v>
+      </c>
+      <c r="U18" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="V18" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="W18" s="4">
+        <v>0.19</v>
+      </c>
     </row>
     <row r="19" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
@@ -1687,11 +1708,17 @@
         <v>0.82</v>
       </c>
       <c r="T19" s="4">
-        <v>0.79</v>
-      </c>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
+        <v>0.78</v>
+      </c>
+      <c r="U19" s="4">
+        <v>0.71</v>
+      </c>
+      <c r="V19" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="W19" s="4">
+        <v>0.63</v>
+      </c>
     </row>
     <row r="20" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
@@ -1752,11 +1779,17 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="T20" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
+        <v>0.09</v>
+      </c>
+      <c r="U20" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="V20" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="W20" s="4">
+        <v>0.19</v>
+      </c>
     </row>
     <row r="21" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="5" t="s">
@@ -1819,9 +1852,15 @@
       <c r="T21" s="4">
         <v>0</v>
       </c>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
+      <c r="U21" s="4">
+        <v>0</v>
+      </c>
+      <c r="V21" s="4">
+        <v>0</v>
+      </c>
+      <c r="W21" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:23" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C22" s="1" t="s">
@@ -1873,6 +1912,18 @@
         <v>45</v>
       </c>
       <c r="S22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W22" s="1" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>